<commit_message>
feat: Add scripts for Portuguese fact-checking dataset handling and translation
</commit_message>
<xml_diff>
--- a/resultados2/metrics_por_modelo_com_baseline.xlsx
+++ b/resultados2/metrics_por_modelo_com_baseline.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,88 +468,110 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BERT-base</t>
+          <t>'que'</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5.451584036861147</v>
+        <v>7.408005850655692e-07</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2525377046334437</v>
+        <v>0.2459704509873425</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5720309262485765</v>
+        <v>0.5328279916121972</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1528486394557823</v>
+        <v>0.1139455782312925</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5879157607604004</v>
+        <v>0.9142857142857144</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DistilBERT</t>
+          <t>BERT-base</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.514832104955401</v>
+        <v>11.17942175694874</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2518782416452667</v>
+        <v>0.2591049582795449</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6147445391511906</v>
+        <v>0.6112338608849558</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1432823129251701</v>
+        <v>0.1917517006802721</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2238313191070968</v>
+        <v>0.2615458072350867</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Original</t>
+          <t>DistilBERT</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1.425894728728703</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0.2518782416452667</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.6147445391511906</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0.1432823129251701</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2356209741053671</v>
+        <v>0.2238313191070968</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Original</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.2356209741053671</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>SBERT-MiniLM</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>0.6115248118128095</v>
-      </c>
-      <c r="C5" t="n">
+      <c r="B6" t="n">
+        <v>0.5699858495167324</v>
+      </c>
+      <c r="C6" t="n">
         <v>0.2658867488076567</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D6" t="n">
         <v>0.6353943151502961</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E6" t="n">
         <v>0.2144274376417234</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F6" t="n">
         <v>0.2500094726066669</v>
       </c>
     </row>

</xml_diff>